<commit_message>
update to add arduino code, other misc CAD
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malac\Documents\GitHub\Dauber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51677DB0-A777-4E74-B820-E3FAA5389CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ABF6BE-EA10-4776-8C49-C1C7973596A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="240" windowWidth="28695" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical Parts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="108">
   <si>
     <t>Quantity</t>
   </si>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>Carbon Steel</t>
+  </si>
+  <si>
+    <t>Quoted Price from Sinorise</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Received?</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -493,7 +505,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -502,7 +514,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -511,6 +523,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -793,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,9 +822,10 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -836,8 +850,11 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -863,8 +880,11 @@
       <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -890,8 +910,11 @@
       <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -917,8 +940,11 @@
       <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -944,8 +970,11 @@
       <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -971,8 +1000,11 @@
       <c r="H6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -998,8 +1030,11 @@
       <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1025,8 +1060,11 @@
       <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1052,8 +1090,11 @@
       <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1079,8 +1120,11 @@
       <c r="H10" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1106,8 +1150,11 @@
       <c r="H11" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1133,8 +1180,11 @@
       <c r="H12" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1160,8 +1210,11 @@
       <c r="H13" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1187,8 +1240,11 @@
       <c r="H14" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1214,8 +1270,11 @@
       <c r="H15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1241,8 +1300,11 @@
       <c r="H16" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1268,8 +1330,11 @@
       <c r="H17" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1295,8 +1360,11 @@
       <c r="H18" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -1322,8 +1390,11 @@
       <c r="H19" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1349,85 +1420,88 @@
       <c r="H20" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
@@ -1548,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B4665F-3E49-4D7F-8336-B6CC2E0EF0FF}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,9 +1638,10 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1591,8 +1666,11 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1618,8 +1696,11 @@
       <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1645,8 +1726,11 @@
       <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1672,8 +1756,11 @@
       <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1699,8 +1786,11 @@
       <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1726,8 +1816,11 @@
       <c r="H6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1753,8 +1846,11 @@
       <c r="H7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1780,8 +1876,11 @@
       <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1807,50 +1906,53 @@
       <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="1"/>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="1"/>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
@@ -2072,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87A3320-38FA-43BB-BB29-639CA17EB87B}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,9 +2185,10 @@
     <col min="1" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>83</v>
       </c>
@@ -2095,8 +2198,11 @@
       <c r="D2" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>85</v>
       </c>
@@ -2106,8 +2212,11 @@
       <c r="D3" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>86</v>
       </c>
@@ -2117,8 +2226,11 @@
       <c r="D4" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>87</v>
       </c>
@@ -2128,8 +2240,11 @@
       <c r="D5" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>88</v>
       </c>
@@ -2139,8 +2254,11 @@
       <c r="D6" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>89</v>
       </c>
@@ -2150,8 +2268,11 @@
       <c r="D7" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>90</v>
       </c>
@@ -2161,8 +2282,11 @@
       <c r="D8" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>91</v>
       </c>
@@ -2172,8 +2296,11 @@
       <c r="D9" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>92</v>
       </c>
@@ -2183,8 +2310,11 @@
       <c r="D10" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>93</v>
       </c>
@@ -2194,8 +2324,11 @@
       <c r="D11" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>94</v>
       </c>
@@ -2205,8 +2338,11 @@
       <c r="D12" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>95</v>
       </c>
@@ -2216,8 +2352,11 @@
       <c r="D13" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>96</v>
       </c>
@@ -2227,8 +2366,11 @@
       <c r="D14" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>97</v>
       </c>
@@ -2238,8 +2380,11 @@
       <c r="D15" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>98</v>
       </c>
@@ -2249,8 +2394,11 @@
       <c r="D16" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>99</v>
       </c>
@@ -2260,8 +2408,11 @@
       <c r="D17" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>100</v>
       </c>
@@ -2271,8 +2422,11 @@
       <c r="D18" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>101</v>
       </c>
@@ -2281,6 +2435,18 @@
       </c>
       <c r="D19" s="12" t="s">
         <v>103</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(F3:F19)</f>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>